<commit_message>
Testfälle hinzugefügt, Code cleanup
</commit_message>
<xml_diff>
--- a/Testfälle.xlsx
+++ b/Testfälle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\xampp\htdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F254BE60-DC84-4A39-9B95-822A0DA222FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6D514E-F575-4436-8D94-327834F1316D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F15858BB-909D-408B-AD9C-C7696F132AB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F15858BB-909D-408B-AD9C-C7696F132AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Testfall</t>
   </si>
@@ -114,6 +114,42 @@
   </si>
   <si>
     <t>Beispielsdatensatz bearbeiten</t>
+  </si>
+  <si>
+    <t>Wann wird dies getestet?</t>
+  </si>
+  <si>
+    <t>Beim Aufruf der Seite</t>
+  </si>
+  <si>
+    <t>Beim Klick des Buttons</t>
+  </si>
+  <si>
+    <t>Wenn das Feld nicht ausgefüllt ist</t>
+  </si>
+  <si>
+    <t>Wenn ein falscher Wert eingefügt wird</t>
+  </si>
+  <si>
+    <t>Toast beim Entfernen</t>
+  </si>
+  <si>
+    <t>Beim Klick auf Entfernen</t>
+  </si>
+  <si>
+    <t>Callback von Ajax Call</t>
+  </si>
+  <si>
+    <t>Toast wird angezeigt</t>
+  </si>
+  <si>
+    <t>Toast beim Hinzufügen</t>
+  </si>
+  <si>
+    <t>Beim Speichern des Formulars</t>
+  </si>
+  <si>
+    <t>Toast beim Bearbeiten</t>
   </si>
 </sst>
 </file>
@@ -500,197 +536,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65F9AE7-DB9E-4E75-82FF-64A7F2BE430D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="str">
         <f>"@media im CSS des Frameworks"</f>
         <v>@media im CSS des Frameworks</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="str">
         <f>"@media im CSS des Frameworks"</f>
         <v>@media im CSS des Frameworks</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="str">
         <f>"@media im CSS des Frameworks"</f>
         <v>@media im CSS des Frameworks</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="str">
         <f>"@media im CSS des Frameworks"</f>
         <v>@media im CSS des Frameworks</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E12" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E3 E9:E1048576">
+  <conditionalFormatting sqref="F1:F3 F12:F1048576">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Fehlerhaft"</formula>
     </cfRule>
@@ -698,7 +825,7 @@
       <formula>"Erfolgreich"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E8">
+  <conditionalFormatting sqref="F4:F11">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Fehlerhaft"</formula>
     </cfRule>

</xml_diff>